<commit_message>
Fixed priors to toybox configuration; very quick output, reasonable r hat
</commit_message>
<xml_diff>
--- a/manuscript/data/BayesianFitForecast/output/SIRV_two_strain-Influenza-negativebinomial-cal-17-fcst-10/convergence-SIRV_two_strain-Influenza-negativebinomial-cal-17-fcst-10.xlsx
+++ b/manuscript/data/BayesianFitForecast/output/SIRV_two_strain-Influenza-negativebinomial-cal-17-fcst-10/convergence-SIRV_two_strain-Influenza-negativebinomial-cal-17-fcst-10.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Calibration</t>
   </si>
@@ -35,46 +35,34 @@
     <t xml:space="preserve">Rhat</t>
   </si>
   <si>
-    <t xml:space="preserve">Lambda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( 1.44246841734914e+305 , 1.7252487477451e+305 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beta1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( 0.2 , 0.49 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beta2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( 0.27 , 0.5 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mu</t>
+    <t xml:space="preserve">gamma1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( 0 , 0.02 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gamma2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( 0.05 , 0.1 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu</t>
   </si>
   <si>
     <t xml:space="preserve">( 0 , 0 )</t>
   </si>
   <si>
-    <t xml:space="preserve">gamma1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( 0.19 , 0.26 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gamma2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( 0.18 , 0.3 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nu</t>
+    <t xml:space="preserve">rho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( 0.06 , 0.7 )</t>
   </si>
   <si>
     <t xml:space="preserve">phi1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( 0.19 , 0.33 )</t>
   </si>
   <si>
     <t xml:space="preserve">phi2</t>
@@ -440,19 +428,19 @@
         <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>1.60604972881589e+305</v>
+        <v>0.01</v>
       </c>
       <c r="D2" t="n">
-        <v>1.62824087508457e+305</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G2" t="e">
-        <v>#NUM!</v>
+      <c r="F2" t="n">
+        <v>2624.7</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -463,19 +451,19 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.37</v>
+        <v>0.09</v>
       </c>
       <c r="D3" t="n">
-        <v>0.39</v>
+        <v>0.09</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>2923.43</v>
       </c>
       <c r="G3" t="n">
-        <v>3510407005.41</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -486,19 +474,19 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.41</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1693.7</v>
       </c>
       <c r="G4" t="n">
-        <v>1841294794.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -509,19 +497,19 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>2425.17</v>
       </c>
       <c r="G5" t="n">
-        <v>69089674.08</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -532,19 +520,19 @@
         <v>15</v>
       </c>
       <c r="C6" t="n">
-        <v>0.21</v>
+        <v>0.25</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>2516.06</v>
       </c>
       <c r="G6" t="n">
-        <v>1205747656.53</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -555,88 +543,19 @@
         <v>17</v>
       </c>
       <c r="C7" t="n">
-        <v>0.26</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.28</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>3197.5</v>
       </c>
       <c r="G7" t="n">
-        <v>1865894773.55</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1667254068.07</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" t="n">
-        <v>60660749.22</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" t="n">
-        <v>55150960.15</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated output with new equation
</commit_message>
<xml_diff>
--- a/manuscript/data/BayesianFitForecast/output/SIRV_two_strain-Influenza-negativebinomial-cal-17-fcst-10/convergence-SIRV_two_strain-Influenza-negativebinomial-cal-17-fcst-10.xlsx
+++ b/manuscript/data/BayesianFitForecast/output/SIRV_two_strain-Influenza-negativebinomial-cal-17-fcst-10/convergence-SIRV_two_strain-Influenza-negativebinomial-cal-17-fcst-10.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Calibration</t>
   </si>
@@ -35,16 +35,28 @@
     <t xml:space="preserve">Rhat</t>
   </si>
   <si>
+    <t xml:space="preserve">beta1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( 0.84 , 1.06 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beta2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( 0.04 , 1.43 )</t>
+  </si>
+  <si>
     <t xml:space="preserve">gamma1</t>
   </si>
   <si>
-    <t xml:space="preserve">( 0 , 0.02 )</t>
+    <t xml:space="preserve">( 0.15 , 0.34 )</t>
   </si>
   <si>
     <t xml:space="preserve">gamma2</t>
   </si>
   <si>
-    <t xml:space="preserve">( 0.05 , 0.1 )</t>
+    <t xml:space="preserve">( 0.15 , 0.35 )</t>
   </si>
   <si>
     <t xml:space="preserve">nu</t>
@@ -56,13 +68,13 @@
     <t xml:space="preserve">rho</t>
   </si>
   <si>
-    <t xml:space="preserve">( 0.06 , 0.7 )</t>
+    <t xml:space="preserve">( 0.06 , 0.71 )</t>
   </si>
   <si>
     <t xml:space="preserve">phi1</t>
   </si>
   <si>
-    <t xml:space="preserve">( 0.19 , 0.33 )</t>
+    <t xml:space="preserve">( 0.34 , 0.7 )</t>
   </si>
   <si>
     <t xml:space="preserve">phi2</t>
@@ -428,19 +440,19 @@
         <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01</v>
+        <v>0.97</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.97</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="n">
-        <v>2624.7</v>
+        <v>127.9</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="3">
@@ -451,16 +463,16 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.09</v>
+        <v>0.58</v>
       </c>
       <c r="D3" t="n">
-        <v>0.09</v>
+        <v>0.51</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>2923.43</v>
+        <v>797.82</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -474,19 +486,19 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="n">
-        <v>1693.7</v>
+        <v>203.88</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="5">
@@ -497,16 +509,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="D5" t="n">
-        <v>0.32</v>
+        <v>0.25</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="n">
-        <v>2425.17</v>
+        <v>450.36</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -520,19 +532,19 @@
         <v>15</v>
       </c>
       <c r="C6" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
       <c r="F6" t="n">
-        <v>2516.06</v>
+        <v>342.94</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="7">
@@ -543,18 +555,64 @@
         <v>17</v>
       </c>
       <c r="C7" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="n">
+        <v>584.59</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="n">
+        <v>395.88</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="n">
         <v>0</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D9" t="n">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3197.5</v>
-      </c>
-      <c r="G7" t="n">
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="n">
+        <v>631.57</v>
+      </c>
+      <c r="G9" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>